<commit_message>
Update DWA full JR Korrektur
</commit_message>
<xml_diff>
--- a/Data/DWA_full_JR.xlsx
+++ b/Data/DWA_full_JR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julerickert/Documents/DWA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F6ABD0-100B-F147-A96D-7AB6C52015FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3205A941-48D1-1F44-8A26-6AF968BF90F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20791,9 +20791,6 @@
     <t>Loos (w)</t>
   </si>
   <si>
-    <t>&lt;Kennt man hier nicht.&gt;</t>
-  </si>
-  <si>
     <t>Gaisl (w)</t>
   </si>
   <si>
@@ -21364,9 +21361,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>&lt;Zusammengestellt von den Lehrern aufgrund der Angaben der Schüler.&gt;</t>
-  </si>
-  <si>
     <t>Leich (w)</t>
   </si>
   <si>
@@ -21466,9 +21460,6 @@
     <t>S,A</t>
   </si>
   <si>
-    <t>&lt;durch Schüler und Erwachsene des Dorfes.&gt;</t>
-  </si>
-  <si>
     <t>amäis</t>
   </si>
   <si>
@@ -21583,9 +21574,6 @@
     <t>Fladermüss (w)</t>
   </si>
   <si>
-    <t>s'Omt (s)</t>
-  </si>
-  <si>
     <t>Gogummere (w)</t>
   </si>
   <si>
@@ -21688,9 +21676,6 @@
     <t>Kienzheim</t>
   </si>
   <si>
-    <t>&lt;Wanner, Daniel, Zimmer, Karl.&gt;</t>
-  </si>
-  <si>
     <t>Ameise</t>
   </si>
   <si>
@@ -21817,9 +21802,6 @@
     <t>Eckert Heinrich</t>
   </si>
   <si>
-    <t>&lt;erfragt bei 12 bis 17 jährigen&gt;</t>
-  </si>
-  <si>
     <t>Ämäse (w)</t>
   </si>
   <si>
@@ -21961,9 +21943,6 @@
     <t>Heinrich Ammann</t>
   </si>
   <si>
-    <t>&lt;Lehrer, Schüler und Eingeborene.&gt;</t>
-  </si>
-  <si>
     <t>Ohmeise</t>
   </si>
   <si>
@@ -22078,9 +22057,6 @@
     <t>Lo[e]s, Sau</t>
   </si>
   <si>
-    <t>Göttle &lt;(Patin)&gt;, Pfedderich &lt;(Pate)&gt;</t>
-  </si>
-  <si>
     <t>Peitsch, Geißel</t>
   </si>
   <si>
@@ -22121,6 +22097,30 @@
   </si>
   <si>
     <t xml:space="preserve">Schüssel </t>
+  </si>
+  <si>
+    <t>durch Schüler und Erwachsene des Dorfes.</t>
+  </si>
+  <si>
+    <t>Wanner, Daniel, Zimmer, Karl.</t>
+  </si>
+  <si>
+    <t>erfragt bei 12 bis 17 jährigen</t>
+  </si>
+  <si>
+    <t>Lehrer, Schüler und Eingeborene.</t>
+  </si>
+  <si>
+    <t>Zusammengestellt von den Lehrern aufgrund der Angaben der Schüler.</t>
+  </si>
+  <si>
+    <t>Omt (s', s)</t>
+  </si>
+  <si>
+    <t>nb</t>
+  </si>
+  <si>
+    <t>Pfedderich</t>
   </si>
 </sst>
 </file>
@@ -22548,9 +22548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE2566"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1384" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1397" sqref="F1397"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2225" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AZ2276" sqref="AZ2276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -85983,7 +85983,7 @@
         <v>48.878839999999997</v>
       </c>
       <c r="K2169" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2169">
         <v>24.4</v>
@@ -85992,11 +85992,14 @@
         <v>48.5</v>
       </c>
       <c r="N2169" t="s">
-        <v>6938</v>
+        <v>6937</v>
       </c>
       <c r="O2169" t="s">
         <v>3840</v>
       </c>
+      <c r="P2169">
+        <v>999</v>
+      </c>
       <c r="Q2169" t="s">
         <v>4352</v>
       </c>
@@ -86004,7 +86007,7 @@
         <v>6827</v>
       </c>
       <c r="S2169" t="s">
-        <v>6939</v>
+        <v>6938</v>
       </c>
       <c r="T2169" t="s">
         <v>5674</v>
@@ -86013,106 +86016,106 @@
         <v>999</v>
       </c>
       <c r="V2169" t="s">
-        <v>7356</v>
+        <v>7348</v>
       </c>
       <c r="W2169" t="s">
+        <v>6939</v>
+      </c>
+      <c r="Y2169" t="s">
         <v>6940</v>
       </c>
-      <c r="Y2169" t="s">
+      <c r="Z2169" t="s">
         <v>6941</v>
       </c>
-      <c r="Z2169" t="s">
+      <c r="AA2169" t="s">
         <v>6942</v>
       </c>
-      <c r="AA2169" t="s">
+      <c r="AB2169" t="s">
         <v>6943</v>
       </c>
-      <c r="AB2169" t="s">
+      <c r="AC2169" t="s">
         <v>6944</v>
       </c>
-      <c r="AC2169" t="s">
+      <c r="AD2169" t="s">
         <v>6945</v>
       </c>
-      <c r="AD2169" t="s">
+      <c r="AE2169" t="s">
         <v>6946</v>
       </c>
-      <c r="AE2169" t="s">
+      <c r="AF2169" t="s">
         <v>6947</v>
       </c>
-      <c r="AF2169" t="s">
+      <c r="AG2169" t="s">
         <v>6948</v>
       </c>
-      <c r="AG2169" t="s">
+      <c r="AH2169" t="s">
         <v>6949</v>
       </c>
-      <c r="AH2169" t="s">
+      <c r="AI2169" t="s">
         <v>6950</v>
       </c>
-      <c r="AI2169" t="s">
+      <c r="AJ2169" t="s">
         <v>6951</v>
       </c>
-      <c r="AJ2169" t="s">
+      <c r="AK2169" t="s">
         <v>6952</v>
       </c>
-      <c r="AK2169" t="s">
+      <c r="AL2169" t="s">
         <v>6953</v>
-      </c>
-      <c r="AL2169" t="s">
-        <v>6954</v>
       </c>
       <c r="AM2169">
         <v>999</v>
       </c>
       <c r="AN2169" t="s">
+        <v>6954</v>
+      </c>
+      <c r="AO2169" t="s">
         <v>6955</v>
       </c>
-      <c r="AO2169" t="s">
+      <c r="AP2169" t="s">
         <v>6956</v>
       </c>
-      <c r="AP2169" t="s">
+      <c r="AQ2169" t="s">
         <v>6957</v>
       </c>
-      <c r="AQ2169" t="s">
+      <c r="AR2169" t="s">
         <v>6958</v>
       </c>
-      <c r="AR2169" t="s">
+      <c r="AS2169" t="s">
         <v>6959</v>
       </c>
-      <c r="AS2169" t="s">
+      <c r="AT2169" t="s">
         <v>6960</v>
       </c>
-      <c r="AT2169" t="s">
+      <c r="AU2169" t="s">
         <v>6961</v>
       </c>
-      <c r="AU2169" t="s">
+      <c r="AV2169" t="s">
         <v>6962</v>
       </c>
-      <c r="AV2169" t="s">
+      <c r="AW2169" t="s">
         <v>6963</v>
       </c>
-      <c r="AW2169" t="s">
+      <c r="AX2169" t="s">
         <v>6964</v>
       </c>
-      <c r="AX2169" t="s">
+      <c r="AY2169" t="s">
         <v>6965</v>
       </c>
-      <c r="AY2169" t="s">
+      <c r="AZ2169" t="s">
         <v>6966</v>
       </c>
-      <c r="AZ2169" t="s">
+      <c r="BA2169" t="s">
         <v>6967</v>
       </c>
-      <c r="BA2169" t="s">
+      <c r="BB2169" t="s">
         <v>6968</v>
       </c>
-      <c r="BB2169" t="s">
+      <c r="BC2169" t="s">
         <v>6969</v>
       </c>
-      <c r="BC2169" t="s">
+      <c r="BD2169" t="s">
         <v>6970</v>
-      </c>
-      <c r="BD2169" t="s">
-        <v>6971</v>
       </c>
     </row>
     <row r="2170" spans="2:56" x14ac:dyDescent="0.2">
@@ -86170,7 +86173,7 @@
         <v>48.878689999999999</v>
       </c>
       <c r="K2171" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2171">
         <v>24.4</v>
@@ -86179,7 +86182,7 @@
         <v>48.5</v>
       </c>
       <c r="N2171" t="s">
-        <v>6972</v>
+        <v>6971</v>
       </c>
       <c r="O2171" t="s">
         <v>3846</v>
@@ -86191,7 +86194,7 @@
         <v>999</v>
       </c>
       <c r="S2171" t="s">
-        <v>6973</v>
+        <v>6972</v>
       </c>
       <c r="T2171" t="s">
         <v>4261</v>
@@ -86206,85 +86209,85 @@
         <v>999</v>
       </c>
       <c r="Y2171" t="s">
+        <v>6973</v>
+      </c>
+      <c r="Z2171" t="s">
         <v>6974</v>
       </c>
-      <c r="Z2171" t="s">
+      <c r="AA2171" t="s">
+        <v>6942</v>
+      </c>
+      <c r="AB2171" t="s">
         <v>6975</v>
-      </c>
-      <c r="AA2171" t="s">
-        <v>6943</v>
-      </c>
-      <c r="AB2171" t="s">
-        <v>6976</v>
       </c>
       <c r="AC2171" t="s">
         <v>6880</v>
       </c>
       <c r="AD2171" t="s">
+        <v>6976</v>
+      </c>
+      <c r="AE2171" t="s">
         <v>6977</v>
-      </c>
-      <c r="AE2171" t="s">
-        <v>6978</v>
       </c>
       <c r="AF2171" t="s">
         <v>6882</v>
       </c>
       <c r="AG2171" t="s">
+        <v>6978</v>
+      </c>
+      <c r="AH2171" t="s">
         <v>6979</v>
       </c>
-      <c r="AH2171" t="s">
+      <c r="AI2171" t="s">
         <v>6980</v>
       </c>
-      <c r="AI2171" t="s">
+      <c r="AJ2171" t="s">
         <v>6981</v>
       </c>
-      <c r="AJ2171" t="s">
+      <c r="AK2171" t="s">
         <v>6982</v>
       </c>
-      <c r="AK2171" t="s">
+      <c r="AL2171" t="s">
         <v>6983</v>
       </c>
-      <c r="AL2171" t="s">
+      <c r="AM2171" t="s">
         <v>6984</v>
       </c>
-      <c r="AM2171" t="s">
+      <c r="AN2171" t="s">
         <v>6985</v>
       </c>
-      <c r="AN2171" t="s">
+      <c r="AO2171" t="s">
         <v>6986</v>
-      </c>
-      <c r="AO2171" t="s">
-        <v>6987</v>
       </c>
       <c r="AP2171" t="s">
         <v>6890</v>
       </c>
       <c r="AQ2171" t="s">
+        <v>6987</v>
+      </c>
+      <c r="AR2171" t="s">
         <v>6988</v>
       </c>
-      <c r="AR2171" t="s">
+      <c r="AS2171" t="s">
         <v>6989</v>
       </c>
-      <c r="AS2171" t="s">
+      <c r="AT2171" t="s">
         <v>6990</v>
-      </c>
-      <c r="AT2171" t="s">
-        <v>6991</v>
       </c>
       <c r="AU2171" t="s">
         <v>6893</v>
       </c>
       <c r="AV2171" t="s">
+        <v>6991</v>
+      </c>
+      <c r="AW2171" t="s">
         <v>6992</v>
       </c>
-      <c r="AW2171" t="s">
+      <c r="AX2171" t="s">
         <v>6993</v>
       </c>
-      <c r="AX2171" t="s">
+      <c r="AY2171" t="s">
         <v>6994</v>
-      </c>
-      <c r="AY2171" t="s">
-        <v>6995</v>
       </c>
       <c r="AZ2171">
         <v>999</v>
@@ -86293,13 +86296,13 @@
         <v>999</v>
       </c>
       <c r="BB2171" t="s">
+        <v>6995</v>
+      </c>
+      <c r="BC2171" t="s">
         <v>6996</v>
       </c>
-      <c r="BC2171" t="s">
-        <v>6997</v>
-      </c>
       <c r="BD2171" t="s">
-        <v>6931</v>
+        <v>6930</v>
       </c>
     </row>
     <row r="2172" spans="2:56" x14ac:dyDescent="0.2">
@@ -86357,7 +86360,7 @@
         <v>48.894869999999997</v>
       </c>
       <c r="K2173" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2173">
         <v>24.4</v>
@@ -86366,22 +86369,25 @@
         <v>48.5</v>
       </c>
       <c r="N2173" t="s">
-        <v>6998</v>
+        <v>6997</v>
       </c>
       <c r="O2173" t="s">
         <v>3852</v>
       </c>
+      <c r="P2173">
+        <v>999</v>
+      </c>
       <c r="Q2173" t="s">
-        <v>6999</v>
+        <v>6998</v>
       </c>
       <c r="R2173" t="s">
         <v>6836</v>
       </c>
       <c r="S2173" t="s">
+        <v>6999</v>
+      </c>
+      <c r="T2173" t="s">
         <v>7000</v>
-      </c>
-      <c r="T2173" t="s">
-        <v>7001</v>
       </c>
       <c r="U2173">
         <v>999</v>
@@ -86390,88 +86396,88 @@
         <v>999</v>
       </c>
       <c r="W2173" t="s">
-        <v>7357</v>
+        <v>7349</v>
       </c>
       <c r="Y2173" t="s">
+        <v>7001</v>
+      </c>
+      <c r="Z2173" t="s">
         <v>7002</v>
       </c>
-      <c r="Z2173" t="s">
+      <c r="AA2173" t="s">
         <v>7003</v>
       </c>
-      <c r="AA2173" t="s">
+      <c r="AB2173" t="s">
         <v>7004</v>
       </c>
-      <c r="AB2173" t="s">
+      <c r="AC2173" t="s">
         <v>7005</v>
       </c>
-      <c r="AC2173" t="s">
+      <c r="AD2173" t="s">
         <v>7006</v>
       </c>
-      <c r="AD2173" t="s">
+      <c r="AE2173" t="s">
         <v>7007</v>
       </c>
-      <c r="AE2173" t="s">
+      <c r="AF2173" t="s">
         <v>7008</v>
       </c>
-      <c r="AF2173" t="s">
+      <c r="AG2173" t="s">
         <v>7009</v>
       </c>
-      <c r="AG2173" t="s">
+      <c r="AH2173" t="s">
         <v>7010</v>
       </c>
-      <c r="AH2173" t="s">
+      <c r="AI2173" t="s">
         <v>7011</v>
       </c>
-      <c r="AI2173" t="s">
+      <c r="AJ2173" t="s">
         <v>7012</v>
       </c>
-      <c r="AJ2173" t="s">
+      <c r="AK2173" t="s">
         <v>7013</v>
       </c>
-      <c r="AK2173" t="s">
+      <c r="AL2173" t="s">
         <v>7014</v>
       </c>
-      <c r="AL2173" t="s">
+      <c r="AM2173" t="s">
         <v>7015</v>
       </c>
-      <c r="AM2173" t="s">
+      <c r="AN2173" t="s">
         <v>7016</v>
       </c>
-      <c r="AN2173" t="s">
+      <c r="AO2173" t="s">
         <v>7017</v>
-      </c>
-      <c r="AO2173" t="s">
-        <v>7018</v>
       </c>
       <c r="AP2173" t="s">
         <v>6890</v>
       </c>
       <c r="AQ2173" t="s">
+        <v>7018</v>
+      </c>
+      <c r="AR2173" t="s">
+        <v>6988</v>
+      </c>
+      <c r="AS2173" t="s">
         <v>7019</v>
       </c>
-      <c r="AR2173" t="s">
-        <v>6989</v>
-      </c>
-      <c r="AS2173" t="s">
+      <c r="AT2173" t="s">
+        <v>6921</v>
+      </c>
+      <c r="AU2173" t="s">
         <v>7020</v>
       </c>
-      <c r="AT2173" t="s">
-        <v>6922</v>
-      </c>
-      <c r="AU2173" t="s">
+      <c r="AV2173" t="s">
         <v>7021</v>
       </c>
-      <c r="AV2173" t="s">
+      <c r="AW2173" t="s">
         <v>7022</v>
       </c>
-      <c r="AW2173" t="s">
+      <c r="AX2173" t="s">
         <v>7023</v>
       </c>
-      <c r="AX2173" t="s">
+      <c r="AY2173" t="s">
         <v>7024</v>
-      </c>
-      <c r="AY2173" t="s">
-        <v>7025</v>
       </c>
       <c r="AZ2173">
         <v>999</v>
@@ -86480,13 +86486,13 @@
         <v>999</v>
       </c>
       <c r="BB2173" t="s">
-        <v>7026</v>
+        <v>7025</v>
       </c>
       <c r="BC2173" t="s">
-        <v>6997</v>
+        <v>6996</v>
       </c>
       <c r="BD2173" t="s">
-        <v>7358</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="2174" spans="2:56" x14ac:dyDescent="0.2">
@@ -86518,7 +86524,7 @@
         <v>48.881709999999998</v>
       </c>
       <c r="K2174" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2174">
         <v>24.4</v>
@@ -86527,22 +86533,25 @@
         <v>48.5</v>
       </c>
       <c r="N2174" t="s">
-        <v>7027</v>
+        <v>7026</v>
       </c>
       <c r="O2174" t="s">
         <v>3855</v>
       </c>
+      <c r="P2174">
+        <v>999</v>
+      </c>
       <c r="Q2174" t="s">
-        <v>6999</v>
+        <v>6998</v>
       </c>
       <c r="R2174" t="s">
         <v>6827</v>
       </c>
       <c r="S2174" t="s">
+        <v>7027</v>
+      </c>
+      <c r="T2174" t="s">
         <v>7028</v>
-      </c>
-      <c r="T2174" t="s">
-        <v>7029</v>
       </c>
       <c r="U2174">
         <v>999</v>
@@ -86551,91 +86560,91 @@
         <v>999</v>
       </c>
       <c r="W2174" t="s">
-        <v>6940</v>
+        <v>6939</v>
       </c>
       <c r="X2174" s="9" t="s">
+        <v>7029</v>
+      </c>
+      <c r="Y2174" t="s">
         <v>7030</v>
       </c>
-      <c r="Y2174" t="s">
+      <c r="Z2174" t="s">
+        <v>6941</v>
+      </c>
+      <c r="AA2174" t="s">
+        <v>6942</v>
+      </c>
+      <c r="AB2174" t="s">
         <v>7031</v>
       </c>
-      <c r="Z2174" t="s">
-        <v>6942</v>
-      </c>
-      <c r="AA2174" t="s">
-        <v>6943</v>
-      </c>
-      <c r="AB2174" t="s">
+      <c r="AC2174" t="s">
         <v>7032</v>
       </c>
-      <c r="AC2174" t="s">
+      <c r="AD2174" t="s">
         <v>7033</v>
       </c>
-      <c r="AD2174" t="s">
+      <c r="AE2174" t="s">
         <v>7034</v>
       </c>
-      <c r="AE2174" t="s">
+      <c r="AF2174" t="s">
         <v>7035</v>
       </c>
-      <c r="AF2174" t="s">
+      <c r="AG2174" t="s">
+        <v>6948</v>
+      </c>
+      <c r="AH2174" t="s">
         <v>7036</v>
       </c>
-      <c r="AG2174" t="s">
-        <v>6949</v>
-      </c>
-      <c r="AH2174" t="s">
+      <c r="AI2174" t="s">
         <v>7037</v>
       </c>
-      <c r="AI2174" t="s">
+      <c r="AJ2174" t="s">
         <v>7038</v>
       </c>
-      <c r="AJ2174" t="s">
+      <c r="AK2174" t="s">
         <v>7039</v>
       </c>
-      <c r="AK2174" t="s">
+      <c r="AL2174" t="s">
         <v>7040</v>
       </c>
-      <c r="AL2174" t="s">
+      <c r="AM2174" t="s">
         <v>7041</v>
       </c>
-      <c r="AM2174" t="s">
+      <c r="AN2174" t="s">
         <v>7042</v>
       </c>
-      <c r="AN2174" t="s">
+      <c r="AO2174" t="s">
         <v>7043</v>
       </c>
-      <c r="AO2174" t="s">
+      <c r="AP2174" t="s">
         <v>7044</v>
       </c>
-      <c r="AP2174" t="s">
+      <c r="AQ2174" t="s">
+        <v>6957</v>
+      </c>
+      <c r="AR2174" t="s">
+        <v>6958</v>
+      </c>
+      <c r="AS2174" t="s">
         <v>7045</v>
       </c>
-      <c r="AQ2174" t="s">
-        <v>6958</v>
-      </c>
-      <c r="AR2174" t="s">
-        <v>6959</v>
-      </c>
-      <c r="AS2174" t="s">
+      <c r="AT2174" t="s">
+        <v>6921</v>
+      </c>
+      <c r="AU2174" t="s">
+        <v>6961</v>
+      </c>
+      <c r="AV2174" t="s">
         <v>7046</v>
       </c>
-      <c r="AT2174" t="s">
-        <v>6922</v>
-      </c>
-      <c r="AU2174" t="s">
-        <v>6962</v>
-      </c>
-      <c r="AV2174" t="s">
+      <c r="AW2174" t="s">
         <v>7047</v>
       </c>
-      <c r="AW2174" t="s">
+      <c r="AX2174" t="s">
         <v>7048</v>
       </c>
-      <c r="AX2174" t="s">
+      <c r="AY2174" t="s">
         <v>7049</v>
-      </c>
-      <c r="AY2174" t="s">
-        <v>7050</v>
       </c>
       <c r="AZ2174">
         <v>999</v>
@@ -86644,13 +86653,13 @@
         <v>999</v>
       </c>
       <c r="BB2174" t="s">
+        <v>7050</v>
+      </c>
+      <c r="BC2174" t="s">
         <v>7051</v>
       </c>
-      <c r="BC2174" t="s">
+      <c r="BD2174" t="s">
         <v>7052</v>
-      </c>
-      <c r="BD2174" t="s">
-        <v>7053</v>
       </c>
     </row>
     <row r="2175" spans="2:56" x14ac:dyDescent="0.2">
@@ -87618,7 +87627,7 @@
         <v>48.87312</v>
       </c>
       <c r="K2211" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2211">
         <v>25.1</v>
@@ -87627,11 +87636,14 @@
         <v>48.5</v>
       </c>
       <c r="N2211" t="s">
-        <v>7054</v>
+        <v>7053</v>
       </c>
       <c r="O2211" t="s">
         <v>3960</v>
       </c>
+      <c r="P2211">
+        <v>999</v>
+      </c>
       <c r="Q2211" t="s">
         <v>4352</v>
       </c>
@@ -87651,7 +87663,7 @@
         <v>999</v>
       </c>
       <c r="W2211" t="s">
-        <v>6934</v>
+        <v>6933</v>
       </c>
       <c r="Y2211">
         <v>999</v>
@@ -88715,7 +88727,7 @@
         <v>48.882489999999997</v>
       </c>
       <c r="K2248" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2248">
         <v>25.4</v>
@@ -88724,11 +88736,14 @@
         <v>48.5</v>
       </c>
       <c r="N2248" t="s">
-        <v>6937</v>
+        <v>6936</v>
       </c>
       <c r="O2248" t="s">
         <v>4065</v>
       </c>
+      <c r="P2248">
+        <v>999</v>
+      </c>
       <c r="Q2248" t="s">
         <v>4110</v>
       </c>
@@ -88736,10 +88751,10 @@
         <v>4833</v>
       </c>
       <c r="S2248" t="s">
+        <v>6931</v>
+      </c>
+      <c r="T2248" t="s">
         <v>6932</v>
-      </c>
-      <c r="T2248" t="s">
-        <v>6933</v>
       </c>
       <c r="U2248">
         <v>999</v>
@@ -88748,7 +88763,7 @@
         <v>999</v>
       </c>
       <c r="W2248" t="s">
-        <v>6935</v>
+        <v>6934</v>
       </c>
       <c r="Y2248" t="s">
         <v>6901</v>
@@ -88805,46 +88820,46 @@
         <v>6918</v>
       </c>
       <c r="AQ2248" t="s">
+        <v>7361</v>
+      </c>
+      <c r="AR2248" t="s">
         <v>6919</v>
       </c>
-      <c r="AR2248" t="s">
+      <c r="AS2248" t="s">
         <v>6920</v>
       </c>
-      <c r="AS2248" t="s">
+      <c r="AT2248" t="s">
         <v>6921</v>
       </c>
-      <c r="AT2248" t="s">
+      <c r="AU2248" t="s">
         <v>6922</v>
       </c>
-      <c r="AU2248" t="s">
+      <c r="AV2248" t="s">
         <v>6923</v>
       </c>
-      <c r="AV2248" t="s">
+      <c r="AW2248" t="s">
         <v>6924</v>
       </c>
-      <c r="AW2248" t="s">
+      <c r="AX2248" t="s">
         <v>6925</v>
-      </c>
-      <c r="AX2248" t="s">
-        <v>6926</v>
       </c>
       <c r="AY2248">
         <v>999</v>
       </c>
       <c r="AZ2248" t="s">
+        <v>6926</v>
+      </c>
+      <c r="BA2248" t="s">
         <v>6927</v>
       </c>
-      <c r="BA2248" t="s">
+      <c r="BB2248" t="s">
         <v>6928</v>
       </c>
-      <c r="BB2248" t="s">
+      <c r="BC2248" t="s">
         <v>6929</v>
       </c>
-      <c r="BC2248" t="s">
+      <c r="BD2248" t="s">
         <v>6930</v>
-      </c>
-      <c r="BD2248" t="s">
-        <v>6931</v>
       </c>
     </row>
     <row r="2249" spans="2:56" x14ac:dyDescent="0.2">
@@ -89032,7 +89047,7 @@
         <v>48.900449999999999</v>
       </c>
       <c r="K2255" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2255">
         <v>550</v>
@@ -89041,11 +89056,14 @@
         <v>850</v>
       </c>
       <c r="N2255" t="s">
-        <v>7055</v>
+        <v>7054</v>
       </c>
       <c r="O2255" t="s">
         <v>4084</v>
       </c>
+      <c r="P2255">
+        <v>999</v>
+      </c>
       <c r="Q2255" t="s">
         <v>4110</v>
       </c>
@@ -89053,10 +89071,10 @@
         <v>4825</v>
       </c>
       <c r="S2255" t="s">
+        <v>7055</v>
+      </c>
+      <c r="T2255" t="s">
         <v>7056</v>
-      </c>
-      <c r="T2255" t="s">
-        <v>7057</v>
       </c>
       <c r="U2255">
         <v>999</v>
@@ -89065,103 +89083,103 @@
         <v>999</v>
       </c>
       <c r="W2255" t="s">
-        <v>6940</v>
+        <v>6939</v>
       </c>
       <c r="Y2255" t="s">
+        <v>7057</v>
+      </c>
+      <c r="Z2255" t="s">
         <v>7058</v>
       </c>
-      <c r="Z2255" t="s">
+      <c r="AA2255" t="s">
         <v>7059</v>
       </c>
-      <c r="AA2255" t="s">
+      <c r="AB2255" t="s">
         <v>7060</v>
       </c>
-      <c r="AB2255" t="s">
+      <c r="AC2255" t="s">
         <v>7061</v>
       </c>
-      <c r="AC2255" t="s">
+      <c r="AD2255" t="s">
+        <v>7033</v>
+      </c>
+      <c r="AE2255" t="s">
         <v>7062</v>
       </c>
-      <c r="AD2255" t="s">
-        <v>7034</v>
-      </c>
-      <c r="AE2255" t="s">
+      <c r="AF2255" t="s">
         <v>7063</v>
       </c>
-      <c r="AF2255" t="s">
+      <c r="AG2255" t="s">
         <v>7064</v>
       </c>
-      <c r="AG2255" t="s">
+      <c r="AH2255" t="s">
         <v>7065</v>
       </c>
-      <c r="AH2255" t="s">
+      <c r="AI2255" t="s">
         <v>7066</v>
       </c>
-      <c r="AI2255" t="s">
+      <c r="AJ2255" t="s">
         <v>7067</v>
       </c>
-      <c r="AJ2255" t="s">
+      <c r="AK2255" t="s">
         <v>7068</v>
       </c>
-      <c r="AK2255" t="s">
+      <c r="AL2255" t="s">
+        <v>6983</v>
+      </c>
+      <c r="AM2255" t="s">
         <v>7069</v>
       </c>
-      <c r="AL2255" t="s">
-        <v>6984</v>
-      </c>
-      <c r="AM2255" t="s">
+      <c r="AN2255" t="s">
         <v>7070</v>
       </c>
-      <c r="AN2255" t="s">
+      <c r="AO2255" t="s">
         <v>7071</v>
-      </c>
-      <c r="AO2255" t="s">
-        <v>7072</v>
       </c>
       <c r="AP2255" t="s">
         <v>6918</v>
       </c>
       <c r="AQ2255" t="s">
+        <v>7072</v>
+      </c>
+      <c r="AR2255" t="s">
         <v>7073</v>
       </c>
-      <c r="AR2255" t="s">
+      <c r="AS2255" t="s">
         <v>7074</v>
       </c>
-      <c r="AS2255" t="s">
+      <c r="AT2255" t="s">
         <v>7075</v>
-      </c>
-      <c r="AT2255" t="s">
-        <v>7076</v>
       </c>
       <c r="AU2255" t="s">
         <v>6893</v>
       </c>
       <c r="AV2255" t="s">
+        <v>7076</v>
+      </c>
+      <c r="AW2255" t="s">
         <v>7077</v>
       </c>
-      <c r="AW2255" t="s">
+      <c r="AX2255" t="s">
         <v>7078</v>
-      </c>
-      <c r="AX2255" t="s">
-        <v>7079</v>
       </c>
       <c r="AY2255">
         <v>999</v>
       </c>
       <c r="AZ2255" t="s">
+        <v>7079</v>
+      </c>
+      <c r="BA2255" t="s">
         <v>7080</v>
       </c>
-      <c r="BA2255" t="s">
+      <c r="BB2255" t="s">
         <v>7081</v>
       </c>
-      <c r="BB2255" t="s">
+      <c r="BC2255" t="s">
         <v>7082</v>
       </c>
-      <c r="BC2255" t="s">
-        <v>7083</v>
-      </c>
       <c r="BD2255" t="s">
-        <v>6971</v>
+        <v>6970</v>
       </c>
     </row>
     <row r="2256" spans="2:56" x14ac:dyDescent="0.2">
@@ -89285,6 +89303,9 @@
       <c r="O2259" t="s">
         <v>3238</v>
       </c>
+      <c r="P2259">
+        <v>999</v>
+      </c>
       <c r="Q2259" t="s">
         <v>4110</v>
       </c>
@@ -89292,7 +89313,7 @@
         <v>4833</v>
       </c>
       <c r="S2259" t="s">
-        <v>7084</v>
+        <v>7083</v>
       </c>
       <c r="T2259" t="s">
         <v>4824</v>
@@ -89304,88 +89325,88 @@
         <v>999</v>
       </c>
       <c r="W2259" t="s">
-        <v>6934</v>
+        <v>6933</v>
       </c>
       <c r="Y2259" t="s">
+        <v>7084</v>
+      </c>
+      <c r="Z2259" t="s">
         <v>7085</v>
       </c>
-      <c r="Z2259" t="s">
+      <c r="AA2259" t="s">
         <v>7086</v>
       </c>
-      <c r="AA2259" t="s">
+      <c r="AB2259" t="s">
         <v>7087</v>
       </c>
-      <c r="AB2259" t="s">
+      <c r="AC2259" t="s">
         <v>7088</v>
       </c>
-      <c r="AC2259" t="s">
+      <c r="AD2259" t="s">
         <v>7089</v>
       </c>
-      <c r="AD2259" t="s">
+      <c r="AE2259" t="s">
         <v>7090</v>
-      </c>
-      <c r="AE2259" t="s">
-        <v>7091</v>
       </c>
       <c r="AF2259" t="s">
         <v>6882</v>
       </c>
       <c r="AG2259" t="s">
+        <v>7091</v>
+      </c>
+      <c r="AH2259" t="s">
         <v>7092</v>
       </c>
-      <c r="AH2259" t="s">
+      <c r="AI2259" t="s">
         <v>7093</v>
       </c>
-      <c r="AI2259" t="s">
+      <c r="AJ2259" t="s">
         <v>7094</v>
       </c>
-      <c r="AJ2259" t="s">
+      <c r="AK2259" t="s">
+        <v>6982</v>
+      </c>
+      <c r="AL2259" t="s">
         <v>7095</v>
       </c>
-      <c r="AK2259" t="s">
-        <v>6983</v>
-      </c>
-      <c r="AL2259" t="s">
+      <c r="AM2259" t="s">
         <v>7096</v>
       </c>
-      <c r="AM2259" t="s">
+      <c r="AN2259" t="s">
         <v>7097</v>
       </c>
-      <c r="AN2259" t="s">
+      <c r="AO2259" t="s">
         <v>7098</v>
-      </c>
-      <c r="AO2259" t="s">
-        <v>7099</v>
       </c>
       <c r="AP2259" t="s">
         <v>6918</v>
       </c>
       <c r="AQ2259" t="s">
+        <v>7099</v>
+      </c>
+      <c r="AR2259" t="s">
         <v>7100</v>
       </c>
-      <c r="AR2259" t="s">
+      <c r="AS2259" t="s">
         <v>7101</v>
       </c>
-      <c r="AS2259" t="s">
+      <c r="AT2259" t="s">
+        <v>6960</v>
+      </c>
+      <c r="AU2259" t="s">
         <v>7102</v>
       </c>
-      <c r="AT2259" t="s">
-        <v>6961</v>
-      </c>
-      <c r="AU2259" t="s">
+      <c r="AV2259" t="s">
         <v>7103</v>
       </c>
-      <c r="AV2259" t="s">
+      <c r="AW2259" t="s">
         <v>7104</v>
       </c>
-      <c r="AW2259" t="s">
-        <v>7105</v>
-      </c>
       <c r="AX2259" t="s">
-        <v>6965</v>
+        <v>6964</v>
       </c>
       <c r="AY2259" t="s">
-        <v>6995</v>
+        <v>6994</v>
       </c>
       <c r="AZ2259">
         <v>999</v>
@@ -89394,13 +89415,13 @@
         <v>999</v>
       </c>
       <c r="BB2259" t="s">
-        <v>6929</v>
+        <v>6928</v>
       </c>
       <c r="BC2259" t="s">
+        <v>7105</v>
+      </c>
+      <c r="BD2259" t="s">
         <v>7106</v>
-      </c>
-      <c r="BD2259" t="s">
-        <v>7107</v>
       </c>
     </row>
     <row r="2260" spans="2:56" x14ac:dyDescent="0.2">
@@ -89614,7 +89635,7 @@
         <v>48.857300000000002</v>
       </c>
       <c r="K2267" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2267">
         <v>550</v>
@@ -89623,11 +89644,14 @@
         <v>850</v>
       </c>
       <c r="N2267" t="s">
-        <v>7108</v>
+        <v>7107</v>
       </c>
       <c r="O2267" t="s">
         <v>4110</v>
       </c>
+      <c r="P2267">
+        <v>999</v>
+      </c>
       <c r="Q2267" t="s">
         <v>4110</v>
       </c>
@@ -89647,16 +89671,16 @@
         <v>999</v>
       </c>
       <c r="W2267" t="s">
-        <v>7109</v>
+        <v>7108</v>
       </c>
       <c r="X2267" t="s">
-        <v>7110</v>
+        <v>7359</v>
       </c>
       <c r="Y2267">
         <v>999</v>
       </c>
       <c r="Z2267" t="s">
-        <v>7111</v>
+        <v>7109</v>
       </c>
       <c r="AA2267">
         <v>999</v>
@@ -89668,7 +89692,7 @@
         <v>6880</v>
       </c>
       <c r="AD2267" t="s">
-        <v>7090</v>
+        <v>7089</v>
       </c>
       <c r="AE2267">
         <v>999</v>
@@ -89677,16 +89701,16 @@
         <v>6882</v>
       </c>
       <c r="AG2267" t="s">
-        <v>7112</v>
+        <v>7110</v>
       </c>
       <c r="AH2267" t="s">
-        <v>7113</v>
+        <v>7111</v>
       </c>
       <c r="AI2267">
         <v>999</v>
       </c>
       <c r="AJ2267" t="s">
-        <v>7114</v>
+        <v>7112</v>
       </c>
       <c r="AK2267">
         <v>999</v>
@@ -89695,37 +89719,37 @@
         <v>6886</v>
       </c>
       <c r="AM2267" t="s">
-        <v>7115</v>
+        <v>7113</v>
       </c>
       <c r="AN2267">
         <v>999</v>
       </c>
       <c r="AO2267" t="s">
-        <v>7116</v>
+        <v>7114</v>
       </c>
       <c r="AP2267" t="s">
-        <v>7117</v>
+        <v>7115</v>
       </c>
       <c r="AQ2267">
         <v>999</v>
       </c>
       <c r="AR2267" t="s">
-        <v>7074</v>
+        <v>7073</v>
       </c>
       <c r="AS2267">
         <v>999</v>
       </c>
       <c r="AT2267" t="s">
-        <v>7118</v>
+        <v>7116</v>
       </c>
       <c r="AU2267" t="s">
         <v>6893</v>
       </c>
       <c r="AV2267" t="s">
-        <v>7119</v>
+        <v>7117</v>
       </c>
       <c r="AW2267" t="s">
-        <v>7120</v>
+        <v>7118</v>
       </c>
       <c r="AX2267">
         <v>999</v>
@@ -89734,19 +89758,19 @@
         <v>999</v>
       </c>
       <c r="AZ2267" t="s">
-        <v>7121</v>
+        <v>7119</v>
       </c>
       <c r="BA2267" t="s">
-        <v>7122</v>
+        <v>7120</v>
       </c>
       <c r="BB2267" t="s">
         <v>6895</v>
       </c>
       <c r="BC2267" t="s">
-        <v>7123</v>
+        <v>7121</v>
       </c>
       <c r="BD2267" t="s">
-        <v>6931</v>
+        <v>6930</v>
       </c>
     </row>
     <row r="2268" spans="2:56" x14ac:dyDescent="0.2">
@@ -90376,7 +90400,7 @@
         <v>48.813310000000001</v>
       </c>
       <c r="K2291" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2291">
         <v>25.1</v>
@@ -90385,11 +90409,14 @@
         <v>48.45</v>
       </c>
       <c r="N2291" t="s">
-        <v>7124</v>
+        <v>7122</v>
       </c>
       <c r="O2291" t="s">
         <v>4177</v>
       </c>
+      <c r="P2291">
+        <v>999</v>
+      </c>
       <c r="Q2291" t="s">
         <v>4352</v>
       </c>
@@ -90397,31 +90424,31 @@
         <v>6737</v>
       </c>
       <c r="S2291" t="s">
-        <v>7125</v>
+        <v>7123</v>
       </c>
       <c r="T2291" t="s">
         <v>3900</v>
       </c>
       <c r="U2291" t="s">
-        <v>7359</v>
+        <v>7351</v>
       </c>
       <c r="V2291">
         <v>999</v>
       </c>
       <c r="W2291" t="s">
-        <v>6934</v>
+        <v>6933</v>
       </c>
       <c r="Y2291" t="s">
-        <v>7126</v>
+        <v>7124</v>
       </c>
       <c r="Z2291" t="s">
         <v>6878</v>
       </c>
       <c r="AA2291" t="s">
-        <v>7127</v>
+        <v>7125</v>
       </c>
       <c r="AB2291" t="s">
-        <v>7128</v>
+        <v>7126</v>
       </c>
       <c r="AC2291" t="s">
         <v>6880</v>
@@ -90430,7 +90457,7 @@
         <v>999</v>
       </c>
       <c r="AE2291" t="s">
-        <v>7129</v>
+        <v>7127</v>
       </c>
       <c r="AF2291" t="s">
         <v>6882</v>
@@ -90442,25 +90469,25 @@
         <v>6884</v>
       </c>
       <c r="AI2291" t="s">
+        <v>7128</v>
+      </c>
+      <c r="AJ2291" t="s">
+        <v>7129</v>
+      </c>
+      <c r="AK2291" t="s">
+        <v>6982</v>
+      </c>
+      <c r="AL2291" t="s">
+        <v>6983</v>
+      </c>
+      <c r="AM2291" t="s">
         <v>7130</v>
       </c>
-      <c r="AJ2291" t="s">
+      <c r="AN2291" t="s">
         <v>7131</v>
       </c>
-      <c r="AK2291" t="s">
-        <v>6983</v>
-      </c>
-      <c r="AL2291" t="s">
-        <v>6984</v>
-      </c>
-      <c r="AM2291" t="s">
+      <c r="AO2291" t="s">
         <v>7132</v>
-      </c>
-      <c r="AN2291" t="s">
-        <v>7133</v>
-      </c>
-      <c r="AO2291" t="s">
-        <v>7134</v>
       </c>
       <c r="AP2291" t="s">
         <v>6890</v>
@@ -90472,37 +90499,37 @@
         <v>6892</v>
       </c>
       <c r="AS2291" t="s">
-        <v>7135</v>
+        <v>7133</v>
       </c>
       <c r="AT2291" t="s">
-        <v>7136</v>
+        <v>7134</v>
       </c>
       <c r="AU2291" t="s">
         <v>6893</v>
       </c>
       <c r="AV2291" t="s">
+        <v>7135</v>
+      </c>
+      <c r="AW2291" t="s">
+        <v>7136</v>
+      </c>
+      <c r="AX2291" t="s">
+        <v>6993</v>
+      </c>
+      <c r="AY2291">
+        <v>999</v>
+      </c>
+      <c r="AZ2291" t="s">
         <v>7137</v>
-      </c>
-      <c r="AW2291" t="s">
-        <v>7138</v>
-      </c>
-      <c r="AX2291" t="s">
-        <v>6994</v>
-      </c>
-      <c r="AY2291" t="s">
-        <v>7139</v>
-      </c>
-      <c r="AZ2291">
-        <v>999</v>
       </c>
       <c r="BA2291">
         <v>999</v>
       </c>
       <c r="BB2291" t="s">
-        <v>7139</v>
+        <v>7137</v>
       </c>
       <c r="BC2291" t="s">
-        <v>7140</v>
+        <v>7138</v>
       </c>
       <c r="BD2291" t="s">
         <v>6897</v>
@@ -90797,7 +90824,7 @@
         <v>48.802219999999998</v>
       </c>
       <c r="K2302" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2302">
         <v>25.1</v>
@@ -90806,11 +90833,14 @@
         <v>48.45</v>
       </c>
       <c r="N2302" t="s">
-        <v>7141</v>
+        <v>7139</v>
       </c>
       <c r="O2302" t="s">
         <v>4208</v>
       </c>
+      <c r="P2302">
+        <v>999</v>
+      </c>
       <c r="Q2302" t="s">
         <v>4231</v>
       </c>
@@ -90818,7 +90848,7 @@
         <v>6827</v>
       </c>
       <c r="S2302" t="s">
-        <v>7142</v>
+        <v>7140</v>
       </c>
       <c r="T2302" t="s">
         <v>549</v>
@@ -90830,106 +90860,106 @@
         <v>4825</v>
       </c>
       <c r="W2302" t="s">
+        <v>7141</v>
+      </c>
+      <c r="X2302" s="9" t="s">
+        <v>7355</v>
+      </c>
+      <c r="Y2302" t="s">
+        <v>7142</v>
+      </c>
+      <c r="Z2302" t="s">
         <v>7143</v>
       </c>
-      <c r="X2302" s="9" t="s">
+      <c r="AA2302" t="s">
         <v>7144</v>
       </c>
-      <c r="Y2302" t="s">
+      <c r="AB2302" t="s">
         <v>7145</v>
       </c>
-      <c r="Z2302" t="s">
+      <c r="AC2302" t="s">
         <v>7146</v>
       </c>
-      <c r="AA2302" t="s">
+      <c r="AD2302" t="s">
         <v>7147</v>
       </c>
-      <c r="AB2302" t="s">
+      <c r="AE2302" t="s">
         <v>7148</v>
       </c>
-      <c r="AC2302" t="s">
+      <c r="AF2302" t="s">
         <v>7149</v>
       </c>
-      <c r="AD2302" t="s">
+      <c r="AG2302" t="s">
         <v>7150</v>
       </c>
-      <c r="AE2302" t="s">
+      <c r="AH2302" t="s">
         <v>7151</v>
       </c>
-      <c r="AF2302" t="s">
+      <c r="AI2302" t="s">
         <v>7152</v>
       </c>
-      <c r="AG2302" t="s">
+      <c r="AJ2302" t="s">
         <v>7153</v>
       </c>
-      <c r="AH2302" t="s">
+      <c r="AK2302" t="s">
         <v>7154</v>
       </c>
-      <c r="AI2302" t="s">
+      <c r="AL2302" t="s">
         <v>7155</v>
       </c>
-      <c r="AJ2302" t="s">
+      <c r="AM2302" t="s">
         <v>7156</v>
       </c>
-      <c r="AK2302" t="s">
+      <c r="AN2302" t="s">
         <v>7157</v>
       </c>
-      <c r="AL2302" t="s">
+      <c r="AO2302" t="s">
         <v>7158</v>
       </c>
-      <c r="AM2302" t="s">
+      <c r="AP2302" t="s">
         <v>7159</v>
       </c>
-      <c r="AN2302" t="s">
+      <c r="AQ2302" t="s">
         <v>7160</v>
       </c>
-      <c r="AO2302" t="s">
+      <c r="AR2302" t="s">
         <v>7161</v>
       </c>
-      <c r="AP2302" t="s">
+      <c r="AS2302" t="s">
         <v>7162</v>
       </c>
-      <c r="AQ2302" t="s">
+      <c r="AT2302" t="s">
+        <v>6921</v>
+      </c>
+      <c r="AU2302" t="s">
         <v>7163</v>
       </c>
-      <c r="AR2302" t="s">
+      <c r="AV2302" t="s">
         <v>7164</v>
       </c>
-      <c r="AS2302" t="s">
+      <c r="AW2302" t="s">
         <v>7165</v>
       </c>
-      <c r="AT2302" t="s">
-        <v>6922</v>
-      </c>
-      <c r="AU2302" t="s">
+      <c r="AX2302" t="s">
         <v>7166</v>
-      </c>
-      <c r="AV2302" t="s">
-        <v>7167</v>
-      </c>
-      <c r="AW2302" t="s">
-        <v>7168</v>
-      </c>
-      <c r="AX2302" t="s">
-        <v>7169</v>
       </c>
       <c r="AY2302">
         <v>999</v>
       </c>
       <c r="AZ2302" t="s">
+        <v>7167</v>
+      </c>
+      <c r="BA2302" t="s">
+        <v>7168</v>
+      </c>
+      <c r="BB2302" t="s">
+        <v>7169</v>
+      </c>
+      <c r="BC2302" t="s">
+        <v>6969</v>
+      </c>
+      <c r="BD2302" t="s">
         <v>7170</v>
-      </c>
-      <c r="BA2302" t="s">
-        <v>7171</v>
-      </c>
-      <c r="BB2302" t="s">
-        <v>7172</v>
-      </c>
-      <c r="BC2302" t="s">
-        <v>6970</v>
-      </c>
-      <c r="BD2302" t="s">
-        <v>7173</v>
       </c>
     </row>
     <row r="2303" spans="2:56" x14ac:dyDescent="0.2">
@@ -91039,7 +91069,7 @@
         <v>48.757350000000002</v>
       </c>
       <c r="K2306" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2306">
         <v>25.1</v>
@@ -91048,11 +91078,14 @@
         <v>48.45</v>
       </c>
       <c r="N2306" t="s">
-        <v>7174</v>
+        <v>7171</v>
       </c>
       <c r="O2306" t="s">
         <v>4220</v>
       </c>
+      <c r="P2306">
+        <v>999</v>
+      </c>
       <c r="Q2306" t="s">
         <v>6843</v>
       </c>
@@ -91060,70 +91093,70 @@
         <v>6737</v>
       </c>
       <c r="S2306" t="s">
-        <v>7175</v>
+        <v>7172</v>
       </c>
       <c r="T2306" t="s">
-        <v>7176</v>
+        <v>7173</v>
       </c>
       <c r="U2306">
         <v>999</v>
       </c>
       <c r="V2306" t="s">
+        <v>7174</v>
+      </c>
+      <c r="W2306" t="s">
+        <v>6933</v>
+      </c>
+      <c r="Y2306" t="s">
+        <v>7175</v>
+      </c>
+      <c r="Z2306" t="s">
+        <v>7176</v>
+      </c>
+      <c r="AA2306" t="s">
         <v>7177</v>
       </c>
-      <c r="W2306" t="s">
-        <v>6934</v>
-      </c>
-      <c r="Y2306" t="s">
-        <v>7178</v>
-      </c>
-      <c r="Z2306" t="s">
-        <v>7179</v>
-      </c>
-      <c r="AA2306" t="s">
-        <v>7180</v>
-      </c>
       <c r="AB2306" t="s">
-        <v>7128</v>
+        <v>7126</v>
       </c>
       <c r="AC2306" t="s">
         <v>6880</v>
       </c>
       <c r="AD2306" t="s">
-        <v>7181</v>
+        <v>7178</v>
       </c>
       <c r="AE2306" t="s">
-        <v>7182</v>
+        <v>7179</v>
       </c>
       <c r="AF2306" t="s">
         <v>6882</v>
       </c>
       <c r="AG2306" t="s">
+        <v>7360</v>
+      </c>
+      <c r="AH2306" t="s">
+        <v>7180</v>
+      </c>
+      <c r="AI2306" t="s">
+        <v>7128</v>
+      </c>
+      <c r="AJ2306" t="s">
+        <v>7181</v>
+      </c>
+      <c r="AK2306" t="s">
+        <v>6982</v>
+      </c>
+      <c r="AL2306" t="s">
+        <v>7182</v>
+      </c>
+      <c r="AM2306" t="s">
         <v>7183</v>
       </c>
-      <c r="AH2306" t="s">
+      <c r="AN2306" t="s">
+        <v>7131</v>
+      </c>
+      <c r="AO2306" t="s">
         <v>7184</v>
-      </c>
-      <c r="AI2306" t="s">
-        <v>7130</v>
-      </c>
-      <c r="AJ2306" t="s">
-        <v>7185</v>
-      </c>
-      <c r="AK2306" t="s">
-        <v>6983</v>
-      </c>
-      <c r="AL2306" t="s">
-        <v>7186</v>
-      </c>
-      <c r="AM2306" t="s">
-        <v>7187</v>
-      </c>
-      <c r="AN2306" t="s">
-        <v>7133</v>
-      </c>
-      <c r="AO2306" t="s">
-        <v>7188</v>
       </c>
       <c r="AP2306" t="s">
         <v>6890</v>
@@ -91135,25 +91168,25 @@
         <v>6892</v>
       </c>
       <c r="AS2306" t="s">
-        <v>7189</v>
+        <v>7185</v>
       </c>
       <c r="AT2306" t="s">
-        <v>7190</v>
+        <v>7186</v>
       </c>
       <c r="AU2306" t="s">
         <v>6893</v>
       </c>
       <c r="AV2306" t="s">
-        <v>7191</v>
+        <v>7187</v>
       </c>
       <c r="AW2306" t="s">
+        <v>6992</v>
+      </c>
+      <c r="AX2306" t="s">
         <v>6993</v>
       </c>
-      <c r="AX2306" t="s">
-        <v>6994</v>
-      </c>
       <c r="AY2306" t="s">
-        <v>7025</v>
+        <v>7024</v>
       </c>
       <c r="AZ2306">
         <v>999</v>
@@ -91162,13 +91195,13 @@
         <v>999</v>
       </c>
       <c r="BB2306" t="s">
-        <v>7192</v>
+        <v>7188</v>
       </c>
       <c r="BC2306" t="s">
-        <v>7193</v>
+        <v>7189</v>
       </c>
       <c r="BD2306" t="s">
-        <v>7194</v>
+        <v>7190</v>
       </c>
     </row>
     <row r="2307" spans="2:56" x14ac:dyDescent="0.2">
@@ -91278,7 +91311,7 @@
         <v>48.814349999999997</v>
       </c>
       <c r="K2310" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2310">
         <v>25.2</v>
@@ -91287,11 +91320,14 @@
         <v>48.45</v>
       </c>
       <c r="N2310" t="s">
-        <v>7195</v>
+        <v>7191</v>
       </c>
       <c r="O2310" t="s">
         <v>4231</v>
       </c>
+      <c r="P2310">
+        <v>999</v>
+      </c>
       <c r="Q2310" t="s">
         <v>4231</v>
       </c>
@@ -91299,7 +91335,7 @@
         <v>6737</v>
       </c>
       <c r="S2310" t="s">
-        <v>7196</v>
+        <v>7192</v>
       </c>
       <c r="T2310" t="s">
         <v>825</v>
@@ -91311,61 +91347,61 @@
         <v>999</v>
       </c>
       <c r="W2310" t="s">
-        <v>6934</v>
+        <v>6933</v>
       </c>
       <c r="Y2310" t="s">
-        <v>7126</v>
+        <v>7124</v>
       </c>
       <c r="Z2310" t="s">
         <v>6878</v>
       </c>
       <c r="AA2310" t="s">
-        <v>7197</v>
+        <v>7193</v>
       </c>
       <c r="AB2310" t="s">
-        <v>7128</v>
+        <v>7126</v>
       </c>
       <c r="AC2310" t="s">
         <v>6880</v>
       </c>
       <c r="AD2310" t="s">
-        <v>7198</v>
+        <v>7194</v>
       </c>
       <c r="AE2310" t="s">
-        <v>7199</v>
+        <v>7195</v>
       </c>
       <c r="AF2310" t="s">
         <v>6882</v>
       </c>
       <c r="AG2310" t="s">
-        <v>7200</v>
+        <v>7196</v>
       </c>
       <c r="AH2310" t="s">
         <v>6884</v>
       </c>
       <c r="AI2310" t="s">
+        <v>7197</v>
+      </c>
+      <c r="AJ2310" t="s">
+        <v>7198</v>
+      </c>
+      <c r="AK2310" t="s">
+        <v>7199</v>
+      </c>
+      <c r="AL2310" t="s">
+        <v>7200</v>
+      </c>
+      <c r="AM2310" t="s">
         <v>7201</v>
       </c>
-      <c r="AJ2310" t="s">
+      <c r="AN2310" t="s">
         <v>7202</v>
       </c>
-      <c r="AK2310" t="s">
+      <c r="AO2310" t="s">
         <v>7203</v>
       </c>
-      <c r="AL2310" t="s">
+      <c r="AP2310" t="s">
         <v>7204</v>
-      </c>
-      <c r="AM2310" t="s">
-        <v>7205</v>
-      </c>
-      <c r="AN2310" t="s">
-        <v>7206</v>
-      </c>
-      <c r="AO2310" t="s">
-        <v>7207</v>
-      </c>
-      <c r="AP2310" t="s">
-        <v>7208</v>
       </c>
       <c r="AQ2310" t="s">
         <v>6891</v>
@@ -91374,25 +91410,25 @@
         <v>6892</v>
       </c>
       <c r="AS2310" t="s">
-        <v>7209</v>
+        <v>7205</v>
       </c>
       <c r="AT2310" t="s">
-        <v>7210</v>
+        <v>7206</v>
       </c>
       <c r="AU2310" t="s">
         <v>6893</v>
       </c>
       <c r="AV2310" t="s">
-        <v>7211</v>
+        <v>7207</v>
       </c>
       <c r="AW2310" t="s">
-        <v>7138</v>
+        <v>7136</v>
       </c>
       <c r="AX2310" t="s">
-        <v>7212</v>
+        <v>7208</v>
       </c>
       <c r="AY2310" t="s">
-        <v>7025</v>
+        <v>7024</v>
       </c>
       <c r="AZ2310">
         <v>999</v>
@@ -91401,10 +91437,10 @@
         <v>999</v>
       </c>
       <c r="BB2310" t="s">
-        <v>7213</v>
+        <v>7209</v>
       </c>
       <c r="BC2310" t="s">
-        <v>7214</v>
+        <v>7210</v>
       </c>
       <c r="BD2310" t="s">
         <v>6897</v>
@@ -91699,7 +91735,7 @@
         <v>48.768259999999998</v>
       </c>
       <c r="K2321" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2321">
         <v>25.3</v>
@@ -91708,11 +91744,14 @@
         <v>48.45</v>
       </c>
       <c r="N2321" t="s">
-        <v>7215</v>
+        <v>7211</v>
       </c>
       <c r="O2321" t="s">
         <v>4261</v>
       </c>
+      <c r="P2321">
+        <v>999</v>
+      </c>
       <c r="Q2321" t="s">
         <v>4231</v>
       </c>
@@ -91720,10 +91759,10 @@
         <v>6737</v>
       </c>
       <c r="S2321" t="s">
-        <v>7216</v>
+        <v>7212</v>
       </c>
       <c r="T2321" t="s">
-        <v>7217</v>
+        <v>7213</v>
       </c>
       <c r="U2321" t="s">
         <v>803</v>
@@ -91732,106 +91771,106 @@
         <v>6737</v>
       </c>
       <c r="W2321" t="s">
-        <v>6934</v>
+        <v>6933</v>
       </c>
       <c r="X2321" s="9" t="s">
+        <v>7356</v>
+      </c>
+      <c r="Y2321" t="s">
+        <v>7214</v>
+      </c>
+      <c r="Z2321" t="s">
+        <v>7215</v>
+      </c>
+      <c r="AA2321" t="s">
+        <v>7216</v>
+      </c>
+      <c r="AB2321" t="s">
+        <v>7031</v>
+      </c>
+      <c r="AC2321" t="s">
+        <v>6944</v>
+      </c>
+      <c r="AD2321" t="s">
+        <v>7217</v>
+      </c>
+      <c r="AE2321" t="s">
         <v>7218</v>
       </c>
-      <c r="Y2321" t="s">
+      <c r="AF2321" t="s">
+        <v>6947</v>
+      </c>
+      <c r="AG2321" t="s">
+        <v>6948</v>
+      </c>
+      <c r="AH2321" t="s">
         <v>7219</v>
       </c>
-      <c r="Z2321" t="s">
+      <c r="AI2321" t="s">
         <v>7220</v>
       </c>
-      <c r="AA2321" t="s">
+      <c r="AJ2321" t="s">
         <v>7221</v>
       </c>
-      <c r="AB2321" t="s">
-        <v>7032</v>
-      </c>
-      <c r="AC2321" t="s">
-        <v>6945</v>
-      </c>
-      <c r="AD2321" t="s">
+      <c r="AK2321" t="s">
         <v>7222</v>
       </c>
-      <c r="AE2321" t="s">
+      <c r="AL2321" t="s">
         <v>7223</v>
       </c>
-      <c r="AF2321" t="s">
-        <v>6948</v>
-      </c>
-      <c r="AG2321" t="s">
-        <v>6949</v>
-      </c>
-      <c r="AH2321" t="s">
+      <c r="AM2321" t="s">
         <v>7224</v>
       </c>
-      <c r="AI2321" t="s">
+      <c r="AN2321" t="s">
         <v>7225</v>
       </c>
-      <c r="AJ2321" t="s">
+      <c r="AO2321" t="s">
         <v>7226</v>
       </c>
-      <c r="AK2321" t="s">
+      <c r="AP2321" t="s">
+        <v>6956</v>
+      </c>
+      <c r="AQ2321" t="s">
         <v>7227</v>
       </c>
-      <c r="AL2321" t="s">
+      <c r="AR2321" t="s">
         <v>7228</v>
       </c>
-      <c r="AM2321" t="s">
+      <c r="AS2321" t="s">
         <v>7229</v>
       </c>
-      <c r="AN2321" t="s">
+      <c r="AT2321" t="s">
         <v>7230</v>
       </c>
-      <c r="AO2321" t="s">
+      <c r="AU2321" t="s">
         <v>7231</v>
       </c>
-      <c r="AP2321" t="s">
-        <v>6957</v>
-      </c>
-      <c r="AQ2321" t="s">
+      <c r="AV2321" t="s">
         <v>7232</v>
       </c>
-      <c r="AR2321" t="s">
+      <c r="AW2321" t="s">
         <v>7233</v>
       </c>
-      <c r="AS2321" t="s">
+      <c r="AX2321" t="s">
         <v>7234</v>
-      </c>
-      <c r="AT2321" t="s">
-        <v>7235</v>
-      </c>
-      <c r="AU2321" t="s">
-        <v>7236</v>
-      </c>
-      <c r="AV2321" t="s">
-        <v>7237</v>
-      </c>
-      <c r="AW2321" t="s">
-        <v>7238</v>
-      </c>
-      <c r="AX2321" t="s">
-        <v>7239</v>
       </c>
       <c r="AY2321">
         <v>999</v>
       </c>
       <c r="AZ2321" t="s">
-        <v>7240</v>
+        <v>7235</v>
       </c>
       <c r="BA2321" t="s">
-        <v>7241</v>
+        <v>7236</v>
       </c>
       <c r="BB2321" t="s">
-        <v>7242</v>
+        <v>7237</v>
       </c>
       <c r="BC2321" t="s">
-        <v>6997</v>
+        <v>6996</v>
       </c>
       <c r="BD2321" t="s">
-        <v>7243</v>
+        <v>7238</v>
       </c>
     </row>
     <row r="2322" spans="2:56" x14ac:dyDescent="0.2">
@@ -91941,7 +91980,7 @@
         <v>48.806600000000003</v>
       </c>
       <c r="K2325" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2325">
         <v>25.3</v>
@@ -91950,11 +91989,14 @@
         <v>48.45</v>
       </c>
       <c r="N2325" t="s">
-        <v>7244</v>
+        <v>7239</v>
       </c>
       <c r="O2325" t="s">
         <v>4273</v>
       </c>
+      <c r="P2325">
+        <v>999</v>
+      </c>
       <c r="Q2325" t="s">
         <v>4231</v>
       </c>
@@ -91962,7 +92004,7 @@
         <v>6737</v>
       </c>
       <c r="S2325" t="s">
-        <v>7245</v>
+        <v>7240</v>
       </c>
       <c r="T2325" t="s">
         <v>6761</v>
@@ -91974,58 +92016,58 @@
         <v>6737</v>
       </c>
       <c r="W2325" t="s">
-        <v>6935</v>
+        <v>6934</v>
       </c>
       <c r="Y2325" t="s">
-        <v>7246</v>
+        <v>7241</v>
       </c>
       <c r="Z2325" t="s">
         <v>6878</v>
       </c>
       <c r="AA2325" t="s">
-        <v>7247</v>
+        <v>7242</v>
       </c>
       <c r="AB2325" t="s">
-        <v>7248</v>
+        <v>7243</v>
       </c>
       <c r="AC2325" t="s">
         <v>6880</v>
       </c>
       <c r="AD2325" t="s">
-        <v>7249</v>
+        <v>7244</v>
       </c>
       <c r="AE2325" t="s">
-        <v>7250</v>
+        <v>7245</v>
       </c>
       <c r="AF2325" t="s">
         <v>6882</v>
       </c>
       <c r="AG2325" t="s">
-        <v>7251</v>
+        <v>7246</v>
       </c>
       <c r="AH2325" t="s">
         <v>6884</v>
       </c>
       <c r="AI2325" t="s">
-        <v>7252</v>
+        <v>7247</v>
       </c>
       <c r="AJ2325" t="s">
-        <v>7253</v>
+        <v>7248</v>
       </c>
       <c r="AK2325" t="s">
-        <v>7254</v>
+        <v>7249</v>
       </c>
       <c r="AL2325" t="s">
-        <v>6984</v>
+        <v>6983</v>
       </c>
       <c r="AM2325" t="s">
-        <v>7205</v>
+        <v>7201</v>
       </c>
       <c r="AN2325" t="s">
-        <v>7255</v>
+        <v>7250</v>
       </c>
       <c r="AO2325" t="s">
-        <v>7256</v>
+        <v>7251</v>
       </c>
       <c r="AP2325" t="s">
         <v>6890</v>
@@ -92034,28 +92076,28 @@
         <v>6891</v>
       </c>
       <c r="AR2325" t="s">
-        <v>7257</v>
+        <v>7252</v>
       </c>
       <c r="AS2325" t="s">
-        <v>7189</v>
+        <v>7185</v>
       </c>
       <c r="AT2325" t="s">
-        <v>6961</v>
+        <v>6960</v>
       </c>
       <c r="AU2325" t="s">
-        <v>7103</v>
+        <v>7102</v>
       </c>
       <c r="AV2325" t="s">
         <v>6894</v>
       </c>
       <c r="AW2325" t="s">
-        <v>7138</v>
+        <v>7136</v>
       </c>
       <c r="AX2325" t="s">
-        <v>6994</v>
+        <v>6993</v>
       </c>
       <c r="AY2325" t="s">
-        <v>7025</v>
+        <v>7024</v>
       </c>
       <c r="AZ2325">
         <v>999</v>
@@ -92064,10 +92106,10 @@
         <v>999</v>
       </c>
       <c r="BB2325" t="s">
-        <v>7258</v>
+        <v>7253</v>
       </c>
       <c r="BC2325" t="s">
-        <v>7106</v>
+        <v>7105</v>
       </c>
       <c r="BD2325" t="s">
         <v>6897</v>
@@ -92154,7 +92196,7 @@
         <v>48.830849999999998</v>
       </c>
       <c r="K2328" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2328">
         <v>25.4</v>
@@ -92163,11 +92205,14 @@
         <v>48.45</v>
       </c>
       <c r="N2328" t="s">
-        <v>7259</v>
+        <v>7254</v>
       </c>
       <c r="O2328" t="s">
         <v>4282</v>
       </c>
+      <c r="P2328">
+        <v>999</v>
+      </c>
       <c r="Q2328" t="s">
         <v>4231</v>
       </c>
@@ -92175,7 +92220,7 @@
         <v>6827</v>
       </c>
       <c r="S2328" t="s">
-        <v>7260</v>
+        <v>7255</v>
       </c>
       <c r="T2328" t="s">
         <v>2779</v>
@@ -92187,91 +92232,91 @@
         <v>999</v>
       </c>
       <c r="W2328" t="s">
-        <v>6940</v>
+        <v>6939</v>
       </c>
       <c r="X2328" s="9" t="s">
+        <v>7357</v>
+      </c>
+      <c r="Y2328" t="s">
+        <v>7256</v>
+      </c>
+      <c r="Z2328" t="s">
+        <v>7257</v>
+      </c>
+      <c r="AA2328" t="s">
+        <v>7258</v>
+      </c>
+      <c r="AB2328" t="s">
+        <v>7259</v>
+      </c>
+      <c r="AC2328" t="s">
+        <v>7260</v>
+      </c>
+      <c r="AD2328" t="s">
         <v>7261</v>
       </c>
-      <c r="Y2328" t="s">
+      <c r="AE2328" t="s">
         <v>7262</v>
       </c>
-      <c r="Z2328" t="s">
+      <c r="AF2328" t="s">
         <v>7263</v>
       </c>
-      <c r="AA2328" t="s">
+      <c r="AG2328" t="s">
         <v>7264</v>
       </c>
-      <c r="AB2328" t="s">
+      <c r="AH2328" t="s">
         <v>7265</v>
       </c>
-      <c r="AC2328" t="s">
+      <c r="AI2328" t="s">
+        <v>7352</v>
+      </c>
+      <c r="AJ2328" t="s">
         <v>7266</v>
       </c>
-      <c r="AD2328" t="s">
+      <c r="AK2328" t="s">
+        <v>6952</v>
+      </c>
+      <c r="AL2328" t="s">
         <v>7267</v>
       </c>
-      <c r="AE2328" t="s">
+      <c r="AM2328" t="s">
+        <v>7130</v>
+      </c>
+      <c r="AN2328" t="s">
+        <v>7250</v>
+      </c>
+      <c r="AO2328" t="s">
         <v>7268</v>
-      </c>
-      <c r="AF2328" t="s">
-        <v>7269</v>
-      </c>
-      <c r="AG2328" t="s">
-        <v>7270</v>
-      </c>
-      <c r="AH2328" t="s">
-        <v>7271</v>
-      </c>
-      <c r="AI2328" t="s">
-        <v>7360</v>
-      </c>
-      <c r="AJ2328" t="s">
-        <v>7272</v>
-      </c>
-      <c r="AK2328" t="s">
-        <v>6953</v>
-      </c>
-      <c r="AL2328" t="s">
-        <v>7273</v>
-      </c>
-      <c r="AM2328" t="s">
-        <v>7132</v>
-      </c>
-      <c r="AN2328" t="s">
-        <v>7255</v>
-      </c>
-      <c r="AO2328" t="s">
-        <v>7274</v>
       </c>
       <c r="AP2328" t="s">
         <v>6890</v>
       </c>
       <c r="AQ2328" t="s">
-        <v>7275</v>
+        <v>7269</v>
       </c>
       <c r="AR2328" t="s">
-        <v>7276</v>
+        <v>7270</v>
       </c>
       <c r="AS2328" t="s">
-        <v>7277</v>
+        <v>7271</v>
       </c>
       <c r="AT2328" t="s">
-        <v>7278</v>
+        <v>7272</v>
       </c>
       <c r="AU2328" t="s">
-        <v>6962</v>
+        <v>6961</v>
       </c>
       <c r="AV2328" t="s">
-        <v>7279</v>
+        <v>7273</v>
       </c>
       <c r="AW2328" t="s">
-        <v>7361</v>
+        <v>7353</v>
       </c>
       <c r="AX2328" t="s">
-        <v>7079</v>
+        <v>7078</v>
       </c>
       <c r="AY2328" t="s">
-        <v>7280</v>
+        <v>7274</v>
       </c>
       <c r="AZ2328">
         <v>999</v>
@@ -92280,13 +92325,13 @@
         <v>999</v>
       </c>
       <c r="BB2328" t="s">
-        <v>7281</v>
+        <v>7275</v>
       </c>
       <c r="BC2328" t="s">
-        <v>7282</v>
+        <v>7276</v>
       </c>
       <c r="BD2328" t="s">
-        <v>7283</v>
+        <v>7277</v>
       </c>
     </row>
     <row r="2329" spans="2:56" x14ac:dyDescent="0.2">
@@ -92370,20 +92415,23 @@
         <v>48.822870000000002</v>
       </c>
       <c r="K2331" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2331">
         <v>540</v>
       </c>
       <c r="M2331" t="s">
-        <v>7284</v>
+        <v>7278</v>
       </c>
       <c r="N2331" t="s">
-        <v>7285</v>
+        <v>7279</v>
       </c>
       <c r="O2331" t="s">
         <v>4291</v>
       </c>
+      <c r="P2331">
+        <v>999</v>
+      </c>
       <c r="Q2331" t="s">
         <v>4110</v>
       </c>
@@ -92391,7 +92439,7 @@
         <v>4825</v>
       </c>
       <c r="S2331" t="s">
-        <v>7286</v>
+        <v>7280</v>
       </c>
       <c r="T2331" t="s">
         <v>5657</v>
@@ -92403,103 +92451,103 @@
         <v>999</v>
       </c>
       <c r="W2331" t="s">
-        <v>6935</v>
+        <v>6934</v>
       </c>
       <c r="Y2331" t="s">
+        <v>7281</v>
+      </c>
+      <c r="Z2331" t="s">
+        <v>7282</v>
+      </c>
+      <c r="AA2331" t="s">
+        <v>7283</v>
+      </c>
+      <c r="AB2331" t="s">
+        <v>7060</v>
+      </c>
+      <c r="AC2331" t="s">
+        <v>7032</v>
+      </c>
+      <c r="AD2331" t="s">
+        <v>7284</v>
+      </c>
+      <c r="AE2331" t="s">
+        <v>7285</v>
+      </c>
+      <c r="AF2331" t="s">
+        <v>6947</v>
+      </c>
+      <c r="AG2331" t="s">
+        <v>7286</v>
+      </c>
+      <c r="AH2331" t="s">
         <v>7287</v>
       </c>
-      <c r="Z2331" t="s">
+      <c r="AI2331" t="s">
         <v>7288</v>
       </c>
-      <c r="AA2331" t="s">
+      <c r="AJ2331" t="s">
         <v>7289</v>
       </c>
-      <c r="AB2331" t="s">
-        <v>7061</v>
-      </c>
-      <c r="AC2331" t="s">
-        <v>7033</v>
-      </c>
-      <c r="AD2331" t="s">
+      <c r="AK2331" t="s">
+        <v>7068</v>
+      </c>
+      <c r="AL2331" t="s">
         <v>7290</v>
       </c>
-      <c r="AE2331" t="s">
+      <c r="AM2331" t="s">
         <v>7291</v>
       </c>
-      <c r="AF2331" t="s">
-        <v>6948</v>
-      </c>
-      <c r="AG2331" t="s">
+      <c r="AN2331" t="s">
         <v>7292</v>
       </c>
-      <c r="AH2331" t="s">
+      <c r="AO2331" t="s">
         <v>7293</v>
       </c>
-      <c r="AI2331" t="s">
+      <c r="AP2331" t="s">
         <v>7294</v>
       </c>
-      <c r="AJ2331" t="s">
+      <c r="AQ2331" t="s">
+        <v>7072</v>
+      </c>
+      <c r="AR2331" t="s">
         <v>7295</v>
       </c>
-      <c r="AK2331" t="s">
-        <v>7069</v>
-      </c>
-      <c r="AL2331" t="s">
+      <c r="AS2331" t="s">
         <v>7296</v>
       </c>
-      <c r="AM2331" t="s">
+      <c r="AT2331" t="s">
+        <v>6990</v>
+      </c>
+      <c r="AU2331" t="s">
+        <v>6961</v>
+      </c>
+      <c r="AV2331" t="s">
         <v>7297</v>
       </c>
-      <c r="AN2331" t="s">
+      <c r="AW2331" t="s">
+        <v>7047</v>
+      </c>
+      <c r="AX2331" t="s">
         <v>7298</v>
       </c>
-      <c r="AO2331" t="s">
-        <v>7299</v>
-      </c>
-      <c r="AP2331" t="s">
-        <v>7300</v>
-      </c>
-      <c r="AQ2331" t="s">
-        <v>7073</v>
-      </c>
-      <c r="AR2331" t="s">
-        <v>7301</v>
-      </c>
-      <c r="AS2331" t="s">
-        <v>7302</v>
-      </c>
-      <c r="AT2331" t="s">
-        <v>6991</v>
-      </c>
-      <c r="AU2331" t="s">
-        <v>6962</v>
-      </c>
-      <c r="AV2331" t="s">
-        <v>7303</v>
-      </c>
-      <c r="AW2331" t="s">
-        <v>7048</v>
-      </c>
-      <c r="AX2331" t="s">
-        <v>7304</v>
-      </c>
-      <c r="AY2331" t="s">
-        <v>7362</v>
-      </c>
-      <c r="AZ2331">
+      <c r="AY2331">
         <v>999</v>
+      </c>
+      <c r="AZ2331" t="s">
+        <v>7354</v>
       </c>
       <c r="BA2331">
         <v>999</v>
       </c>
       <c r="BB2331" t="s">
-        <v>7305</v>
+        <v>7299</v>
       </c>
       <c r="BC2331" t="s">
-        <v>7306</v>
+        <v>7300</v>
       </c>
       <c r="BD2331" t="s">
-        <v>7243</v>
+        <v>7238</v>
       </c>
     </row>
     <row r="2332" spans="2:56" x14ac:dyDescent="0.2">
@@ -92687,7 +92735,7 @@
         <v>48.747169999999997</v>
       </c>
       <c r="K2338" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2338">
         <v>540</v>
@@ -92696,11 +92744,14 @@
         <v>845</v>
       </c>
       <c r="N2338" t="s">
-        <v>7307</v>
+        <v>7301</v>
       </c>
       <c r="O2338" t="s">
         <v>4308</v>
       </c>
+      <c r="P2338">
+        <v>999</v>
+      </c>
       <c r="Q2338" t="s">
         <v>344</v>
       </c>
@@ -92708,7 +92759,7 @@
         <v>4825</v>
       </c>
       <c r="S2338" t="s">
-        <v>7308</v>
+        <v>7302</v>
       </c>
       <c r="T2338" t="s">
         <v>3252</v>
@@ -92720,19 +92771,19 @@
         <v>999</v>
       </c>
       <c r="W2338" t="s">
-        <v>6935</v>
+        <v>6934</v>
       </c>
       <c r="X2338" s="9" t="s">
-        <v>7309</v>
+        <v>7358</v>
       </c>
       <c r="Y2338" t="s">
-        <v>7310</v>
+        <v>7303</v>
       </c>
       <c r="Z2338" t="s">
-        <v>7311</v>
+        <v>7304</v>
       </c>
       <c r="AA2338" t="s">
-        <v>7312</v>
+        <v>7305</v>
       </c>
       <c r="AB2338" t="s">
         <v>6904</v>
@@ -92741,85 +92792,85 @@
         <v>6880</v>
       </c>
       <c r="AD2338" t="s">
-        <v>7313</v>
+        <v>7306</v>
       </c>
       <c r="AE2338" t="s">
-        <v>7314</v>
+        <v>7307</v>
       </c>
       <c r="AF2338" t="s">
         <v>6882</v>
       </c>
       <c r="AG2338" t="s">
+        <v>7308</v>
+      </c>
+      <c r="AH2338" t="s">
+        <v>7309</v>
+      </c>
+      <c r="AI2338" t="s">
+        <v>7093</v>
+      </c>
+      <c r="AJ2338" t="s">
+        <v>7310</v>
+      </c>
+      <c r="AK2338" t="s">
+        <v>6982</v>
+      </c>
+      <c r="AL2338" t="s">
+        <v>7311</v>
+      </c>
+      <c r="AM2338" t="s">
+        <v>7312</v>
+      </c>
+      <c r="AN2338" t="s">
+        <v>7313</v>
+      </c>
+      <c r="AO2338" t="s">
+        <v>7314</v>
+      </c>
+      <c r="AP2338" t="s">
+        <v>7204</v>
+      </c>
+      <c r="AQ2338" t="s">
         <v>7315</v>
       </c>
-      <c r="AH2338" t="s">
+      <c r="AR2338" t="s">
         <v>7316</v>
       </c>
-      <c r="AI2338" t="s">
-        <v>7094</v>
-      </c>
-      <c r="AJ2338" t="s">
+      <c r="AS2338" t="s">
         <v>7317</v>
       </c>
-      <c r="AK2338" t="s">
-        <v>6983</v>
-      </c>
-      <c r="AL2338" t="s">
+      <c r="AT2338" t="s">
         <v>7318</v>
-      </c>
-      <c r="AM2338" t="s">
-        <v>7319</v>
-      </c>
-      <c r="AN2338" t="s">
-        <v>7320</v>
-      </c>
-      <c r="AO2338" t="s">
-        <v>7321</v>
-      </c>
-      <c r="AP2338" t="s">
-        <v>7208</v>
-      </c>
-      <c r="AQ2338" t="s">
-        <v>7322</v>
-      </c>
-      <c r="AR2338" t="s">
-        <v>7323</v>
-      </c>
-      <c r="AS2338" t="s">
-        <v>7324</v>
-      </c>
-      <c r="AT2338" t="s">
-        <v>7325</v>
       </c>
       <c r="AU2338" t="s">
         <v>6893</v>
       </c>
       <c r="AV2338" t="s">
-        <v>7326</v>
+        <v>7319</v>
       </c>
       <c r="AW2338" t="s">
-        <v>7327</v>
+        <v>7320</v>
       </c>
       <c r="AX2338" t="s">
-        <v>6994</v>
+        <v>6993</v>
       </c>
       <c r="AY2338">
         <v>999</v>
       </c>
       <c r="AZ2338" t="s">
-        <v>7328</v>
+        <v>7321</v>
       </c>
       <c r="BA2338" t="s">
-        <v>7329</v>
+        <v>7322</v>
       </c>
       <c r="BB2338" t="s">
-        <v>7330</v>
+        <v>7323</v>
       </c>
       <c r="BC2338" t="s">
-        <v>7331</v>
+        <v>7324</v>
       </c>
       <c r="BD2338" t="s">
-        <v>6931</v>
+        <v>6930</v>
       </c>
     </row>
     <row r="2339" spans="2:56" x14ac:dyDescent="0.2">
@@ -93137,7 +93188,7 @@
         <v>48.76294</v>
       </c>
       <c r="K2350" t="s">
-        <v>6936</v>
+        <v>6935</v>
       </c>
       <c r="L2350">
         <v>25.5</v>
@@ -93146,11 +93197,14 @@
         <v>48.45</v>
       </c>
       <c r="N2350" t="s">
-        <v>7332</v>
+        <v>7325</v>
       </c>
       <c r="O2350" t="s">
         <v>4342</v>
       </c>
+      <c r="P2350">
+        <v>999</v>
+      </c>
       <c r="Q2350" t="s">
         <v>4110</v>
       </c>
@@ -93158,10 +93212,10 @@
         <v>4825</v>
       </c>
       <c r="S2350" t="s">
-        <v>7333</v>
+        <v>7326</v>
       </c>
       <c r="T2350" t="s">
-        <v>7334</v>
+        <v>7327</v>
       </c>
       <c r="U2350">
         <v>999</v>
@@ -93170,103 +93224,103 @@
         <v>999</v>
       </c>
       <c r="W2350" t="s">
-        <v>6935</v>
+        <v>6934</v>
       </c>
       <c r="Y2350" t="s">
-        <v>7287</v>
+        <v>7281</v>
       </c>
       <c r="Z2350" t="s">
+        <v>7328</v>
+      </c>
+      <c r="AA2350" t="s">
+        <v>6942</v>
+      </c>
+      <c r="AB2350" t="s">
+        <v>7329</v>
+      </c>
+      <c r="AC2350" t="s">
+        <v>7330</v>
+      </c>
+      <c r="AD2350" t="s">
+        <v>7331</v>
+      </c>
+      <c r="AE2350" t="s">
+        <v>7332</v>
+      </c>
+      <c r="AF2350" t="s">
+        <v>6947</v>
+      </c>
+      <c r="AG2350" t="s">
+        <v>7333</v>
+      </c>
+      <c r="AH2350" t="s">
+        <v>7334</v>
+      </c>
+      <c r="AI2350" t="s">
+        <v>7288</v>
+      </c>
+      <c r="AJ2350" t="s">
         <v>7335</v>
       </c>
-      <c r="AA2350" t="s">
-        <v>6943</v>
-      </c>
-      <c r="AB2350" t="s">
+      <c r="AK2350" t="s">
         <v>7336</v>
       </c>
-      <c r="AC2350" t="s">
+      <c r="AL2350" t="s">
         <v>7337</v>
       </c>
-      <c r="AD2350" t="s">
+      <c r="AM2350" t="s">
+        <v>7291</v>
+      </c>
+      <c r="AN2350" t="s">
         <v>7338</v>
       </c>
-      <c r="AE2350" t="s">
+      <c r="AO2350" t="s">
         <v>7339</v>
       </c>
-      <c r="AF2350" t="s">
-        <v>6948</v>
-      </c>
-      <c r="AG2350" t="s">
+      <c r="AP2350" t="s">
         <v>7340</v>
       </c>
-      <c r="AH2350" t="s">
+      <c r="AQ2350" t="s">
+        <v>7362</v>
+      </c>
+      <c r="AR2350" t="s">
         <v>7341</v>
       </c>
-      <c r="AI2350" t="s">
-        <v>7294</v>
-      </c>
-      <c r="AJ2350" t="s">
+      <c r="AS2350" t="s">
+        <v>7296</v>
+      </c>
+      <c r="AT2350" t="s">
+        <v>6990</v>
+      </c>
+      <c r="AU2350" t="s">
+        <v>6961</v>
+      </c>
+      <c r="AV2350" t="s">
         <v>7342</v>
       </c>
-      <c r="AK2350" t="s">
+      <c r="AW2350" t="s">
         <v>7343</v>
       </c>
-      <c r="AL2350" t="s">
-        <v>7344</v>
-      </c>
-      <c r="AM2350" t="s">
-        <v>7297</v>
-      </c>
-      <c r="AN2350" t="s">
-        <v>7345</v>
-      </c>
-      <c r="AO2350" t="s">
-        <v>7346</v>
-      </c>
-      <c r="AP2350" t="s">
-        <v>7347</v>
-      </c>
-      <c r="AQ2350" t="s">
-        <v>7348</v>
-      </c>
-      <c r="AR2350" t="s">
-        <v>7349</v>
-      </c>
-      <c r="AS2350" t="s">
-        <v>7302</v>
-      </c>
-      <c r="AT2350" t="s">
-        <v>6991</v>
-      </c>
-      <c r="AU2350" t="s">
-        <v>6962</v>
-      </c>
-      <c r="AV2350" t="s">
-        <v>7350</v>
-      </c>
-      <c r="AW2350" t="s">
-        <v>7351</v>
-      </c>
       <c r="AX2350" t="s">
-        <v>7304</v>
+        <v>7298</v>
       </c>
       <c r="AY2350">
         <v>999</v>
       </c>
       <c r="AZ2350" t="s">
-        <v>7352</v>
+        <v>7344</v>
       </c>
       <c r="BA2350" t="s">
-        <v>7353</v>
+        <v>7345</v>
       </c>
       <c r="BB2350" t="s">
-        <v>7354</v>
+        <v>7346</v>
       </c>
       <c r="BC2350" t="s">
-        <v>7355</v>
+        <v>7347</v>
       </c>
       <c r="BD2350" t="s">
-        <v>6971</v>
+        <v>6970</v>
       </c>
     </row>
     <row r="2351" spans="2:56" x14ac:dyDescent="0.2">

</xml_diff>